<commit_message>
added purchasing list xlsx
</commit_message>
<xml_diff>
--- a/project_finances.xlsx
+++ b/project_finances.xlsx
@@ -164,13 +164,13 @@
     <t>Solder Stand</t>
   </si>
   <si>
-    <t>Paid</t>
-  </si>
-  <si>
     <t>Soldering Filler Metal</t>
   </si>
   <si>
     <t>Wire Stripper</t>
+  </si>
+  <si>
+    <t>Payment Status</t>
   </si>
 </sst>
 </file>
@@ -254,10 +254,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -539,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
+    <sheetView tabSelected="1" topLeftCell="C5" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -558,6 +558,7 @@
     <col min="11" max="11" width="13.5" customWidth="1"/>
     <col min="12" max="12" width="18" style="4" customWidth="1"/>
     <col min="13" max="13" width="18.83203125" style="4" customWidth="1"/>
+    <col min="15" max="15" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
@@ -636,7 +637,7 @@
         <v>34</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
@@ -1144,7 +1145,7 @@
         <v>34</v>
       </c>
       <c r="O22" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -1152,13 +1153,13 @@
         <v>1</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>37</v>
       </c>
       <c r="D23" s="10"/>
-      <c r="E23" s="13">
+      <c r="E23" s="14">
         <v>45</v>
       </c>
       <c r="F23" s="10">
@@ -1168,21 +1169,21 @@
         <v>0</v>
       </c>
       <c r="H23" s="10"/>
-      <c r="I23" s="14">
+      <c r="I23" s="13">
         <f>E23*(1+F23/100)*(1-G23/100)</f>
         <v>45</v>
       </c>
       <c r="J23" s="10">
         <v>20</v>
       </c>
-      <c r="K23" s="14">
+      <c r="K23" s="13">
         <f>I23*J23/100</f>
         <v>9</v>
       </c>
       <c r="L23" s="10">
         <v>80</v>
       </c>
-      <c r="M23" s="14">
+      <c r="M23" s="13">
         <f>I23*L23/100</f>
         <v>36</v>
       </c>
@@ -1216,14 +1217,14 @@
       <c r="J24" s="4">
         <v>20</v>
       </c>
-      <c r="K24" s="14">
+      <c r="K24" s="13">
         <f t="shared" ref="K24:K33" si="4">I24*J24/100</f>
         <v>9.6</v>
       </c>
       <c r="L24" s="4">
         <v>80</v>
       </c>
-      <c r="M24" s="14">
+      <c r="M24" s="13">
         <f t="shared" ref="M24:M33" si="5">I24*L24/100</f>
         <v>38.4</v>
       </c>
@@ -1256,14 +1257,14 @@
       <c r="J25" s="4">
         <v>50</v>
       </c>
-      <c r="K25" s="14">
+      <c r="K25" s="13">
         <f t="shared" si="4"/>
         <v>25.44</v>
       </c>
       <c r="L25" s="4">
         <v>50</v>
       </c>
-      <c r="M25" s="14">
+      <c r="M25" s="13">
         <f t="shared" si="5"/>
         <v>25.44</v>
       </c>
@@ -1299,14 +1300,14 @@
       <c r="J26" s="4">
         <v>20</v>
       </c>
-      <c r="K26" s="14">
+      <c r="K26" s="13">
         <f t="shared" si="4"/>
         <v>0.42400000000000004</v>
       </c>
       <c r="L26" s="4">
         <v>80</v>
       </c>
-      <c r="M26" s="14">
+      <c r="M26" s="13">
         <f t="shared" si="5"/>
         <v>1.6960000000000002</v>
       </c>
@@ -1339,14 +1340,14 @@
       <c r="J27" s="4">
         <v>20</v>
       </c>
-      <c r="K27" s="14">
+      <c r="K27" s="13">
         <f t="shared" si="4"/>
         <v>0.42400000000000004</v>
       </c>
       <c r="L27" s="4">
         <v>80</v>
       </c>
-      <c r="M27" s="14">
+      <c r="M27" s="13">
         <f t="shared" si="5"/>
         <v>1.6960000000000002</v>
       </c>
@@ -1379,14 +1380,14 @@
       <c r="J28" s="4">
         <v>20</v>
       </c>
-      <c r="K28" s="14">
+      <c r="K28" s="13">
         <f t="shared" si="4"/>
         <v>0.42400000000000004</v>
       </c>
       <c r="L28" s="4">
         <v>80</v>
       </c>
-      <c r="M28" s="14">
+      <c r="M28" s="13">
         <f t="shared" si="5"/>
         <v>1.6960000000000002</v>
       </c>
@@ -1419,14 +1420,14 @@
       <c r="J29" s="4">
         <v>20</v>
       </c>
-      <c r="K29" s="14">
+      <c r="K29" s="13">
         <f t="shared" si="4"/>
         <v>3.18</v>
       </c>
       <c r="L29" s="4">
         <v>80</v>
       </c>
-      <c r="M29" s="14">
+      <c r="M29" s="13">
         <f t="shared" si="5"/>
         <v>12.72</v>
       </c>
@@ -1459,14 +1460,14 @@
       <c r="J30" s="4">
         <v>100</v>
       </c>
-      <c r="K30" s="14">
+      <c r="K30" s="13">
         <f t="shared" si="4"/>
         <v>31.8</v>
       </c>
       <c r="L30" s="4">
         <v>0</v>
       </c>
-      <c r="M30" s="14">
+      <c r="M30" s="13">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1499,14 +1500,14 @@
       <c r="J31" s="4">
         <v>80</v>
       </c>
-      <c r="K31" s="14">
+      <c r="K31" s="13">
         <f t="shared" si="4"/>
         <v>6.7840000000000007</v>
       </c>
       <c r="L31" s="4">
         <v>20</v>
       </c>
-      <c r="M31" s="14">
+      <c r="M31" s="13">
         <f t="shared" si="5"/>
         <v>1.6960000000000002</v>
       </c>
@@ -1539,16 +1540,16 @@
       <c r="J32" s="4">
         <v>80</v>
       </c>
-      <c r="K32" s="14">
+      <c r="K32" s="13">
         <f t="shared" si="4"/>
         <v>8.48</v>
       </c>
       <c r="L32" s="4">
-        <v>80</v>
-      </c>
-      <c r="M32" s="14">
+        <v>20</v>
+      </c>
+      <c r="M32" s="13">
         <f t="shared" si="5"/>
-        <v>8.48</v>
+        <v>2.12</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
@@ -1556,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>33</v>
@@ -1579,14 +1580,14 @@
       <c r="J33" s="4">
         <v>50</v>
       </c>
-      <c r="K33" s="14">
+      <c r="K33" s="13">
         <f t="shared" si="4"/>
         <v>3.4449999999999998</v>
       </c>
       <c r="L33" s="4">
         <v>50</v>
       </c>
-      <c r="M33" s="14">
+      <c r="M33" s="13">
         <f t="shared" si="5"/>
         <v>3.4449999999999998</v>
       </c>
@@ -1615,7 +1616,7 @@
       </c>
       <c r="M34" s="7">
         <f>SUM(M23:M33)</f>
-        <v>131.26900000000001</v>
+        <v>124.90899999999999</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>